<commit_message>
This Is Why We Don't Push To Production On Fridays
</commit_message>
<xml_diff>
--- a/data/Modelo Relacional.xlsx
+++ b/data/Modelo Relacional.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="84">
   <si>
     <t>Hotel</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Habitacion</t>
   </si>
   <si>
-    <t>reservado</t>
-  </si>
-  <si>
     <t>descuento</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Number</t>
   </si>
   <si>
-    <t>fecha_inicial</t>
-  </si>
-  <si>
     <t>cargado_habitacion</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>PK, IN (PASAPORTE, CEDULA)</t>
   </si>
   <si>
-    <t>varchar(100)</t>
-  </si>
-  <si>
     <t>tipo_usuario</t>
   </si>
   <si>
@@ -170,9 +161,6 @@
     <t>Plan_Consumo</t>
   </si>
   <si>
-    <t>correo</t>
-  </si>
-  <si>
     <t>num_personas</t>
   </si>
   <si>
@@ -260,9 +248,6 @@
     <t>salida</t>
   </si>
   <si>
-    <t>tipo_servicio</t>
-  </si>
-  <si>
     <t>id_convencion</t>
   </si>
   <si>
@@ -276,6 +261,24 @@
   </si>
   <si>
     <t>id_plan_consumo</t>
+  </si>
+  <si>
+    <t>FK(tipo_servicio.id)</t>
+  </si>
+  <si>
+    <t>id_tipo_servicios</t>
+  </si>
+  <si>
+    <t>tipo_servicios</t>
+  </si>
+  <si>
+    <t>Reserva_servicio</t>
+  </si>
+  <si>
+    <t>fecha_Final</t>
+  </si>
+  <si>
+    <t>fecha_Inicial</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +358,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF4B084"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -406,7 +415,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -414,8 +423,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -429,14 +440,17 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,15 +756,15 @@
     <col min="18" max="18" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -767,72 +781,60 @@
         <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="N3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -840,36 +842,32 @@
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
       <c r="E4" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="P4" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="Q4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -883,143 +881,120 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1033,69 +1008,78 @@
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -1106,33 +1090,33 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="L20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>9</v>
@@ -1141,10 +1125,10 @@
         <v>9</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>11</v>
@@ -1159,21 +1143,21 @@
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -1184,53 +1168,53 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O26" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -1245,16 +1229,16 @@
         <v>9</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>11</v>
@@ -1274,39 +1258,39 @@
         <v>5</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -1324,27 +1308,24 @@
         <v>12</v>
       </c>
       <c r="L31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>11</v>
@@ -1353,96 +1334,151 @@
         <v>2</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P32" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q32" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="R32" s="9"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P33" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q33" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R33" s="10"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="O34" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P34" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Q34" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R34" s="11"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed the fuck out of #331!
</commit_message>
<xml_diff>
--- a/data/Modelo Relacional.xlsx
+++ b/data/Modelo Relacional.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresjaveirgonzaleztorres/Documents/sistrans/HotelAndes/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\Documents\Andes\CuartoSemestre\Sistrans\HotelAndes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7923B03A-3BCE-4962-84BD-E490E99DA380}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="82">
   <si>
     <t>Hotel</t>
   </si>
@@ -134,9 +135,6 @@
     <t>tipo_usuario</t>
   </si>
   <si>
-    <t>id_hotel</t>
-  </si>
-  <si>
     <t>num_habitacion</t>
   </si>
   <si>
@@ -171,9 +169,6 @@
   </si>
   <si>
     <t>FK(servicio.id)</t>
-  </si>
-  <si>
-    <t>FK(hotel.id)</t>
   </si>
   <si>
     <t>FK(plan_consumo.id)</t>
@@ -284,7 +279,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -317,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,12 +353,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF4B084"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -426,7 +415,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -440,17 +429,16 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,14 +716,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:F38"/>
+    <sheetView tabSelected="1" topLeftCell="I18" zoomScale="80" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32:E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
@@ -756,7 +744,7 @@
     <col min="18" max="18" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -764,7 +752,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -781,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>32</v>
@@ -796,10 +784,10 @@
         <v>34</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -834,7 +822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -842,7 +830,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
       <c r="E4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>5</v>
@@ -853,21 +841,21 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -887,28 +875,28 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -949,52 +937,52 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="L13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1014,7 +1002,7 @@
         <v>11</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>2</v>
@@ -1023,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1052,37 +1040,37 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="N16" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="N16" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="O16" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1101,14 +1089,11 @@
       <c r="F20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="L20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -1127,9 +1112,6 @@
       <c r="F21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>20</v>
-      </c>
       <c r="L21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1137,21 +1119,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>20</v>
@@ -1160,56 +1139,56 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L23" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M23" s="7"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L26" t="s">
         <v>34</v>
       </c>
       <c r="O26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -1253,32 +1232,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="D28" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>20</v>
@@ -1293,7 +1272,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="L29" s="7" t="s">
         <v>5</v>
       </c>
@@ -1303,29 +1282,26 @@
       </c>
       <c r="P29" s="7"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="L31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>11</v>
@@ -1334,20 +1310,20 @@
         <v>2</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>29</v>
       </c>
       <c r="Q32" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R32" s="9"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>18</v>
       </c>
@@ -1360,93 +1336,87 @@
       <c r="D33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="L33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="M33" s="4" t="s">
+      <c r="N33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R33" s="10"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="N33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="R33" s="10"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="B34" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O34" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P34" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q34" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R34" s="11"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>9</v>
@@ -1461,23 +1431,23 @@
         <v>19</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sirve generador de usuarios en convencion
</commit_message>
<xml_diff>
--- a/data/Modelo Relacional.xlsx
+++ b/data/Modelo Relacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\Documents\Andes\CuartoSemestre\Sistrans\HotelAndes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7923B03A-3BCE-4962-84BD-E490E99DA380}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF05892-A137-4647-ADF3-96D694249F57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I18" zoomScale="80" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32:E34"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1178,7 +1178,7 @@
       <c r="I26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J26" s="1" t="s">
         <v>75</v>
       </c>
       <c r="L26" t="s">

</xml_diff>